<commit_message>
Main Version 2 Release
</commit_message>
<xml_diff>
--- a/Main/main_test_cases.xlsx
+++ b/Main/main_test_cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\CPR101\GroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\CPR101\GroupProject\Final Submission V1\2 Final Submission\CPR Group 1 Version 2\CPR Group 1 Version 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDA6A18-EEF9-4066-8737-9C26AFE0FA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB360631-9A75-44B3-B267-388117589EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseMatrix" sheetId="2" r:id="rId1"/>
@@ -82,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{9BB0D239-8B99-416E-B82B-F80BA3E3A192}">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{9BB0D239-8B99-416E-B82B-F80BA3E3A192}">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{E121AF1F-0408-4713-A265-1FEF41AD73A9}">
+    <comment ref="B36" authorId="0" shapeId="0" xr:uid="{E121AF1F-0408-4713-A265-1FEF41AD73A9}">
       <text>
         <r>
           <rPr>
@@ -173,21 +173,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="96">
   <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Expected results</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
     <t>Function</t>
   </si>
   <si>
-    <t>Inputs</t>
+    <t>FAIL</t>
   </si>
   <si>
     <t>Program
@@ -217,25 +214,11 @@
     </r>
   </si>
   <si>
-    <t>Version 1</t>
-  </si>
-  <si>
     <t>Run by:
 Date:</t>
   </si>
   <si>
-    <t>Tester
-Date</t>
-  </si>
-  <si>
     <t>Version 2</t>
-  </si>
-  <si>
-    <t>Version 3</t>
-  </si>
-  <si>
-    <t>Actual result
-if unexpected</t>
   </si>
   <si>
     <t>main.c</t>
@@ -306,6 +289,9 @@
 q
 *** End of Converting Strings to int Demo ***
 Type the int numeric string (q - to quit):*** End of Converting Strings to int Demo ***</t>
+  </si>
+  <si>
+    <t>Program ends as expected with an exit code of 0.</t>
   </si>
   <si>
     <t>void fundamentals();</t>
@@ -496,43 +482,16 @@
     <t>manipulating()</t>
   </si>
   <si>
-    <t>(Positive test case[+])        Entered numbers</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>(Positive test case[+])        Enter special characters</t>
-  </si>
-  <si>
-    <t>Special characters were entered and special character were expected</t>
-  </si>
-  <si>
-    <t>Testing a string that is 79 characters to account for null byte 123oojaosdfa534|Testing a string that is 79 characters to account for null byte asdfasdfdfasfdf</t>
-  </si>
-  <si>
     <t>'(Positive test case[+])          Enter q</t>
   </si>
   <si>
     <t>Program ends and prints out "*** End of Concatenating Strings Demo ***"</t>
   </si>
   <si>
-    <t>Concatenated string is 'Testing a string that is 79 characters to account for null byte 123oojaosdfa534Testing a string that is 79 characters to account for null byte asdfasdfdfasfdf'
-Type the 1st string (q - to quit):</t>
-  </si>
-  <si>
-    <t>Type the 1st string (q - to quit):
-^
-Type the 2nd string:
-a
-Concatenated string is '^a'
-Type the 1st string (q - to q</t>
-  </si>
-  <si>
-    <t>^|a</t>
-  </si>
-  <si>
-    <t>Strings were concatenated successfully because each string entered was within 79 characters to account for the null byte.</t>
+    <t>q is the special key that’s suppposed to end the program.</t>
   </si>
   <si>
     <t>Program ends as expected and goes onto tokenizing();</t>
@@ -541,25 +500,150 @@
     <t>Program ends as expected after pressing q and goes to converting();</t>
   </si>
   <si>
-    <t>When entering positive test cases, (as shown in rows 5-17), program exits with Code 0.</t>
-  </si>
-  <si>
-    <t>TheLazyFox|2</t>
-  </si>
-  <si>
-    <t>Type the character position within the string:
-2
-The character found at 2 position is 'e'</t>
-  </si>
-  <si>
-    <t>A non empty string was requested.  I entered the word TheLazyFox. The next prompt appeared without an error Code, This line was successful.                [T|h|e|L|a|z|y|F|o|x|]                            [0|1|2|3|4|5|6|7|8|9|]</t>
+    <r>
+      <t>(POSITIVE TEST CASE[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>➕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">])  
+------------------------------------
+Type a string (q - to quit):
+</t>
+    </r>
+  </si>
+  <si>
+    <t>theotherside</t>
+  </si>
+  <si>
+    <t>The length is 12</t>
+  </si>
+  <si>
+    <t>The code counted the amount of characters in the string and ouputted the length of the string.</t>
+  </si>
+  <si>
+    <t>Entered nothing, only pressed the enter key</t>
+  </si>
+  <si>
+    <t>The length is 0</t>
+  </si>
+  <si>
+    <t>Can take nothing and still give 0 as character length</t>
+  </si>
+  <si>
+    <t>(Positive test case[+])        Entered a short and simple string</t>
+  </si>
+  <si>
+    <t>I like  | cheese</t>
+  </si>
+  <si>
+    <t>I like cheese</t>
+  </si>
+  <si>
+    <t>Two strings were entered and two strings were expected</t>
+  </si>
+  <si>
+    <t>(Positive test case [+])    Entered a large number then a shorter one</t>
+  </si>
+  <si>
+    <t>123456 | 123</t>
+  </si>
+  <si>
+    <t>String one is greater than 2nd</t>
+  </si>
+  <si>
+    <t>The first string is longer than the second one</t>
+  </si>
+  <si>
+    <t>+ Enter various different strings within range within the range of 15^-307 and 15^-307 (i.e., the size of a double)</t>
+  </si>
+  <si>
+    <t>2|123|8888</t>
+  </si>
+  <si>
+    <t>Converted number is 2.000000
+Type the double numeric string (q - to quit):
+123
+Converted number is 123.000000
+Type the double numeric string (q - to quit):
+8888
+Converted number is 8888.000000
+Type the double numeric string (q - to quit):</t>
+  </si>
+  <si>
+    <t>Function will display the converted numerical strings as a double on the screen, so long as the numerical string is within the range of a double.</t>
+  </si>
+  <si>
+    <t>- After adding non-int characters (e.g., a-zA-Z!@#$%%^&amp;* etc.) to our string, do we produce a safeguard message?</t>
+  </si>
+  <si>
+    <t>$a|a55</t>
+  </si>
+  <si>
+    <t>Error! Enter numeric values only.
+Type the double numeric string (q - to quit):| Error! Enter numeric values only. Type the double numeric string (q - to quit):</t>
+  </si>
+  <si>
+    <t>Converted number is 0.000000
+Type the double numeric string (q - to quit):
+a55
+Converted number is 0.000000
+Type the double numeric string (q - to quit):</t>
+  </si>
+  <si>
+    <t>No safeguard has been placed to handle non-double characters. See "Expected Result" for a possible error message that can be produced if the user enters a character that is not a number.</t>
+  </si>
+  <si>
+    <t>+ Inputted spaces between commas with nothing else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, , , </t>
+  </si>
+  <si>
+    <t>Phrase $1 is ' '
+Phrase $2 is ' '
+Phrase $3 is ' '</t>
+  </si>
+  <si>
+    <t>Worked as expected, divided the phrases into different phrases by the comma</t>
+  </si>
+  <si>
+    <t>+ Tested 5 phrases of different lenghts</t>
+  </si>
+  <si>
+    <t>1st, 2nd phrase, The third phrase, This is 4th phrase, This is the 5th phrase</t>
+  </si>
+  <si>
+    <t>Phrase $1 is '1st'
+Phrase $2 is ' 2nd phrase'
+Phrase $3 is ' The third phrase'
+Phrase $4 is ' This is 4th phrase'
+Phrase $5 is ' This is the 5th phrase'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputed series of phrases (5 phrases) of different lenghts (1 word, 2 words, 3 words, 4 words and 5 words respectively). Worked as expected. </t>
+  </si>
+  <si>
+    <t>When entering positive test cases, (as shown in rows 5-25), program exits with Code 0.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -635,6 +719,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -986,7 +1076,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1165,6 +1255,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1177,6 +1270,85 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="7" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="7" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="7" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1195,9 +1367,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1210,25 +1379,70 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1514,10 +1728,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1533,10 +1747,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -1553,30 +1767,30 @@
       <c r="D2" s="38"/>
       <c r="E2" s="56"/>
       <c r="F2" s="34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="24" customFormat="1" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>52</v>
+        <v>5</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>48</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="33" t="s">
         <v>0</v>
@@ -1585,515 +1799,599 @@
     </row>
     <row r="4" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>19</v>
-      </c>
       <c r="G4" s="25" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="H4" s="36"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="77" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="78" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="52" t="s">
-        <v>36</v>
       </c>
       <c r="H5" s="36"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="138" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="47" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D6" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="52" t="s">
         <v>37</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="52" t="s">
-        <v>41</v>
       </c>
       <c r="H6" s="36"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B7" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>76</v>
+      <c r="D7" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>39</v>
       </c>
       <c r="F7" s="51" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="H7" s="36"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="52" t="s">
-        <v>44</v>
+      <c r="A8" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="84" t="s">
+        <v>66</v>
       </c>
       <c r="H8" s="36"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="66" t="s">
+    <row r="9" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="89" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="68" t="s">
-        <v>71</v>
+      <c r="E9" s="87" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="88" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="91" t="s">
+        <v>69</v>
       </c>
       <c r="H9" s="36"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" s="81" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="70" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="75" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="76" t="s">
+    <row r="10" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="36"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="97" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="76" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="76" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="77" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="79"/>
-      <c r="I10" s="80"/>
-    </row>
-    <row r="11" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="71" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="73" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="74" t="s">
+      <c r="C11" s="94" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="93"/>
+      <c r="F11" s="95" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="96" t="s">
         <v>73</v>
       </c>
       <c r="H11" s="36"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="36"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="204" x14ac:dyDescent="0.2">
-      <c r="A14" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="43" t="s">
-        <v>72</v>
+    <row r="12" spans="1:9" s="71" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="99" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="98" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="98" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="98"/>
+      <c r="F12" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="101" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="69"/>
+      <c r="I12" s="70"/>
+    </row>
+    <row r="13" spans="1:9" s="71" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="109" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="107" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="107" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="104"/>
+      <c r="F13" s="108" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="106" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="102"/>
+      <c r="I13" s="103"/>
+    </row>
+    <row r="14" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="68" t="s">
+        <v>62</v>
       </c>
       <c r="H14" s="36"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="204" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
-        <v>45</v>
+    <row r="15" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="39" t="s">
+        <v>15</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="43" t="s">
         <v>19</v>
-      </c>
-      <c r="G15" s="43" t="s">
-        <v>49</v>
       </c>
       <c r="H15" s="36"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
-        <v>45</v>
+    <row r="16" spans="1:9" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="39" t="s">
+        <v>15</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="63" t="s">
-        <v>54</v>
+        <v>21</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>22</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G16" s="43" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="H16" s="36"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="204" x14ac:dyDescent="0.2">
       <c r="A17" s="39" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G17" s="43" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H17" s="36"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
+    <row r="18" spans="1:9" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>81</v>
+      </c>
       <c r="H18" s="36"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
+    <row r="19" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>86</v>
+      </c>
       <c r="H19" s="36"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" s="23" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="24" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="G21" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="31"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="57"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="4"/>
+    <row r="20" spans="1:9" ht="204" x14ac:dyDescent="0.2">
+      <c r="A20" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="36"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" ht="191.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="36"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" s="36"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="57"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="4"/>
+    <row r="23" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="36"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="57"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="4"/>
+    <row r="24" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="111" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="116" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="114" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="113" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="110"/>
+      <c r="F24" s="112" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="115" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="36"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="57"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="4"/>
+    <row r="25" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="118" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="123" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="121" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="120" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="117"/>
+      <c r="F25" s="119" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="122" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="36"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="57"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="4"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="57"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="4"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" s="23" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="24" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="I29" s="31"/>
-    </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="36"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" s="23" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="44"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="35"/>
+    </row>
+    <row r="28" spans="1:9" s="24" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="27"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="33"/>
+      <c r="I28" s="31"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="57"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="4"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="57"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
@@ -2101,7 +2399,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="21"/>
       <c r="G30" s="4"/>
-      <c r="I30" s="1"/>
+      <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="57"/>
@@ -2111,7 +2409,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="21"/>
       <c r="G31" s="4"/>
-      <c r="I31" s="1"/>
+      <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="57"/>
@@ -2121,9 +2419,9 @@
       <c r="E32" s="3"/>
       <c r="F32" s="21"/>
       <c r="G32" s="4"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="57"/>
       <c r="B33" s="9"/>
       <c r="C33" s="10"/>
@@ -2133,61 +2431,130 @@
       <c r="G33" s="4"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="57"/>
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="4"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="21"/>
       <c r="G34" s="4"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="57"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="4"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="57"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="4"/>
-      <c r="I36" s="1"/>
+    <row r="35" spans="1:9" s="23" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="44"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="35"/>
+    </row>
+    <row r="36" spans="1:9" s="24" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="33"/>
+      <c r="I36" s="31"/>
     </row>
     <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="57"/>
       <c r="B37" s="9"/>
       <c r="C37" s="10"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="4"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="3"/>
       <c r="F37" s="21"/>
       <c r="G37" s="4"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="58"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="5"/>
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="57"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="4"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="57"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="4"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="57"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="4"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="57"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="4"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="57"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="4"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="57"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="4"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="57"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="4"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="58"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="5"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A35:E35"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2195,248 +2562,4 @@
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007DA71BB3427D8A4D8C6B1D9FC83B8523" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff806a6af6c9da5df570eefd46bafc37">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="871f9c32-6190-4c20-b083-b734e08baf9d" xmlns:ns3="f9e5404a-8fb4-4d07-81e3-37a7278de386" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="91c5258a233d7e8320f07641405ff8a3" ns2:_="" ns3:_="">
-    <xsd:import namespace="871f9c32-6190-4c20-b083-b734e08baf9d"/>
-    <xsd:import namespace="f9e5404a-8fb4-4d07-81e3-37a7278de386"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="871f9c32-6190-4c20-b083-b734e08baf9d" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f9e5404a-8fb4-4d07-81e3-37a7278de386" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15BBD194-1144-4AEE-9C22-7B8B6DA096FF}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D909448-8367-4803-85D9-110634826A82}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DAFB072-906B-4162-9D24-811822E58683}"/>
 </file>
</xml_diff>